<commit_message>
v0.2 Started work on Experiement1 -Introduce strict -Plan out the experiment -Write up the instructions -Add fluid speed slider -Show force as vector -Print out drag force magnitude -Start on a simple plot of drag vs fluid speed
</commit_message>
<xml_diff>
--- a/cfd todo.xlsx
+++ b/cfd todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Just needs to be the simulation with just the start button for the moment (we'll add the rest of them back in soon)</t>
   </si>
   <si>
@@ -49,10 +52,49 @@
     <t>Introduce strict</t>
   </si>
   <si>
-    <t>Fix those weird edge artifacts at the start</t>
-  </si>
-  <si>
     <t>push v0.1</t>
+  </si>
+  <si>
+    <t>No errors, that's nice.</t>
+  </si>
+  <si>
+    <t>Plan out the experiment</t>
+  </si>
+  <si>
+    <t>Only 8 parts…</t>
+  </si>
+  <si>
+    <t>Write up the instructions</t>
+  </si>
+  <si>
+    <t>Just drafted for the moment</t>
+  </si>
+  <si>
+    <t>Add fluid speed slider</t>
+  </si>
+  <si>
+    <t>Show force as vector</t>
+  </si>
+  <si>
+    <t>Make it red</t>
+  </si>
+  <si>
+    <t>Print out drag force magnitude</t>
+  </si>
+  <si>
+    <t>Bug: Fix those weird edge artifacts at the start</t>
+  </si>
+  <si>
+    <t>Bug: Drag changes with simulation resolution</t>
+  </si>
+  <si>
+    <t>This might be right, not sure?  Could just represent an increase in surface area at higher resolutions.</t>
+  </si>
+  <si>
+    <t>Start on a simple plot of drag vs fluid speed</t>
+  </si>
+  <si>
+    <t>push v0.2</t>
   </si>
 </sst>
 </file>
@@ -82,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,13 +142,34 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -124,35 +187,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -456,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="C13" sqref="C7:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -517,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -529,7 +608,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -540,68 +619,128 @@
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2"/>
+      <c r="A8" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -610,9 +749,15 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,6 +964,30 @@
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
V0.3 - switched to jquery for ui -Auto start simulation on page load -Switch over to jquery ui
</commit_message>
<xml_diff>
--- a/cfd todo.xlsx
+++ b/cfd todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -85,16 +85,31 @@
     <t>Bug: Fix those weird edge artifacts at the start</t>
   </si>
   <si>
-    <t>Bug: Drag changes with simulation resolution</t>
-  </si>
-  <si>
-    <t>This might be right, not sure?  Could just represent an increase in surface area at higher resolutions.</t>
-  </si>
-  <si>
     <t>Start on a simple plot of drag vs fluid speed</t>
   </si>
   <si>
     <t>push v0.2</t>
+  </si>
+  <si>
+    <t>Setup the website on my VPS</t>
+  </si>
+  <si>
+    <t>Setup a process to update the website every push</t>
+  </si>
+  <si>
+    <t>Create a system where user can fit their graph with a linear and square aproximation.</t>
+  </si>
+  <si>
+    <t>Auto start simulation on page load</t>
+  </si>
+  <si>
+    <t>Switch over to jquery ui</t>
+  </si>
+  <si>
+    <t>Looks a lot nicer</t>
+  </si>
+  <si>
+    <t>push v0.3</t>
   </si>
 </sst>
 </file>
@@ -205,7 +220,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -228,6 +243,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -535,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C7:C13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +728,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -724,58 +740,82 @@
         <v>4</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>42427</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,9 +825,15 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -988,6 +1034,36 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bug: case wrong on UI path Change default viscosity to get vortexes quicker Auto plotting of drag vs speed Two experiemnt buttons, one for low speed, one for high Linear regression for low speed experiment
</commit_message>
<xml_diff>
--- a/cfd todo.xlsx
+++ b/cfd todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Setup the website on my VPS</t>
   </si>
   <si>
-    <t>Setup a process to update the website every push</t>
-  </si>
-  <si>
     <t>Create a system where user can fit their graph with a linear and square aproximation.</t>
   </si>
   <si>
@@ -109,7 +106,94 @@
     <t>Looks a lot nicer</t>
   </si>
   <si>
-    <t>push v0.3</t>
+    <t>Bug: case wrong on UI path</t>
+  </si>
+  <si>
+    <t>Stops the css working on linux</t>
+  </si>
+  <si>
+    <t>Handle unstable simulation beter</t>
+  </si>
+  <si>
+    <t>Change default viscosity to get vortexes quicker</t>
+  </si>
+  <si>
+    <t>push</t>
+  </si>
+  <si>
+    <t>V0.3</t>
+  </si>
+  <si>
+    <t>Switch over to jquery for UI</t>
+  </si>
+  <si>
+    <t>V0.2</t>
+  </si>
+  <si>
+    <t>V0.1</t>
+  </si>
+  <si>
+    <t>Intial release</t>
+  </si>
+  <si>
+    <t>Get setup for experiements</t>
+  </si>
+  <si>
+    <t>Improved plotting</t>
+  </si>
+  <si>
+    <t>Clean up UI</t>
+  </si>
+  <si>
+    <t>This is just going to be easyer, call this 'run experiment'</t>
+  </si>
+  <si>
+    <t>Allow configuration of the viscocity</t>
+  </si>
+  <si>
+    <t>Allow selecting of various barrier shapes</t>
+  </si>
+  <si>
+    <t>V0.4</t>
+  </si>
+  <si>
+    <t>Get the graph working properly</t>
+  </si>
+  <si>
+    <t>Right now we plot multiple graphs over top of each other</t>
+  </si>
+  <si>
+    <t>Model fitting</t>
+  </si>
+  <si>
+    <t>V0.5</t>
+  </si>
+  <si>
+    <t>V0.6</t>
+  </si>
+  <si>
+    <t>Code Cleanup and tweaking</t>
+  </si>
+  <si>
+    <t>Works much better, now at 0.2</t>
+  </si>
+  <si>
+    <t>Auto plotting of drag vs speed</t>
+  </si>
+  <si>
+    <t>Two experiemnt buttons, one for low speed, one for high</t>
+  </si>
+  <si>
+    <t>Linear regression for low speed experiment</t>
+  </si>
+  <si>
+    <t>x^2 regression for high speed experiment</t>
+  </si>
+  <si>
+    <t>See if I can make the simulation more stable by taking smaller steps</t>
+  </si>
+  <si>
+    <t>We get unstability quite quick, if I reduce the velocity we loose the non-laminar effect, so I need to have smaller steps, but don't know how to do this.</t>
   </si>
 </sst>
 </file>
@@ -139,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,8 +247,25 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -213,14 +314,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -242,17 +383,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFED"/>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -551,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,30 +750,20 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>42426</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2"/>
+      <c r="A2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>42426</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -612,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -624,9 +785,11 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
@@ -635,8 +798,8 @@
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>12</v>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -648,11 +811,9 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -661,37 +822,25 @@
       <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>42426</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A9" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>42426</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A10" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,10 +851,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,10 +864,12 @@
       <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2"/>
+      <c r="C12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -728,9 +879,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
@@ -739,245 +892,344 @@
       <c r="B14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>24</v>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
-        <v>42427</v>
+        <v>42426</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <v>42428</v>
+        <v>42426</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>28</v>
+      <c r="C16" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
+        <v>42426</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>42426</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>42427</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>42428</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="B22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="2" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="D27" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>42428</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="B28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>42428</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="2"/>
+      <c r="C32" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="2"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="2"/>
+      <c r="A36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="C38" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="2"/>
+      <c r="A46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,21 +1239,31 @@
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="2"/>
+      <c r="A48" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="2"/>
+      <c r="A49" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1011,9 +1273,6 @@
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1064,7 +1323,201 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
V 0.5 Tidy up Seperated out solver code (so I can optimize it later on) Put fluid dynamics stuff into a class to keep it clean, but there's still more work to be done Cleaned up UI a little. Optimized the drawing code (from 4ms to 1ms)
</commit_message>
<xml_diff>
--- a/cfd todo.xlsx
+++ b/cfd todo.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Print out drag force magnitude</t>
   </si>
   <si>
-    <t>Bug: Fix those weird edge artifacts at the start</t>
-  </si>
-  <si>
     <t>Start on a simple plot of drag vs fluid speed</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>Setup the website on my VPS</t>
   </si>
   <si>
-    <t>Create a system where user can fit their graph with a linear and square aproximation.</t>
-  </si>
-  <si>
     <t>Auto start simulation on page load</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>Stops the css working on linux</t>
   </si>
   <si>
-    <t>Handle unstable simulation beter</t>
-  </si>
-  <si>
     <t>Change default viscosity to get vortexes quicker</t>
   </si>
   <si>
@@ -148,33 +139,15 @@
     <t>This is just going to be easyer, call this 'run experiment'</t>
   </si>
   <si>
-    <t>Allow configuration of the viscocity</t>
-  </si>
-  <si>
-    <t>Allow selecting of various barrier shapes</t>
-  </si>
-  <si>
     <t>V0.4</t>
   </si>
   <si>
-    <t>Get the graph working properly</t>
-  </si>
-  <si>
-    <t>Right now we plot multiple graphs over top of each other</t>
-  </si>
-  <si>
-    <t>Model fitting</t>
-  </si>
-  <si>
     <t>V0.5</t>
   </si>
   <si>
     <t>V0.6</t>
   </si>
   <si>
-    <t>Code Cleanup and tweaking</t>
-  </si>
-  <si>
     <t>Works much better, now at 0.2</t>
   </si>
   <si>
@@ -187,13 +160,124 @@
     <t>Linear regression for low speed experiment</t>
   </si>
   <si>
-    <t>x^2 regression for high speed experiment</t>
-  </si>
-  <si>
     <t>See if I can make the simulation more stable by taking smaller steps</t>
   </si>
   <si>
     <t>We get unstability quite quick, if I reduce the velocity we loose the non-laminar effect, so I need to have smaller steps, but don't know how to do this.</t>
+  </si>
+  <si>
+    <t>Tidy up</t>
+  </si>
+  <si>
+    <t>Standard Parts</t>
+  </si>
+  <si>
+    <t>Display a list of selectable parts</t>
+  </si>
+  <si>
+    <t>Allow placing of these parts onto the canvas</t>
+  </si>
+  <si>
+    <t>Use hand to click and drag these parts around</t>
+  </si>
+  <si>
+    <t>V0.7</t>
+  </si>
+  <si>
+    <t>Free form drawing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V0.8 </t>
+  </si>
+  <si>
+    <t>Experiements</t>
+  </si>
+  <si>
+    <t>These are like scenarios, a pre setup experiement with some steps the user must carry out</t>
+  </si>
+  <si>
+    <t>Extra for experts</t>
+  </si>
+  <si>
+    <t>See if I can optimizate the drawing</t>
+  </si>
+  <si>
+    <t>V0.9</t>
+  </si>
+  <si>
+    <t>Mode2</t>
+  </si>
+  <si>
+    <t>In this mode fluid comes out of founts and into wells, and the edges either solid or infinate</t>
+  </si>
+  <si>
+    <t>V0.6.5</t>
+  </si>
+  <si>
+    <t>Instruments</t>
+  </si>
+  <si>
+    <t>Optimization (asm.js, gpu)</t>
+  </si>
+  <si>
+    <t>Able to change simulation speed (very slow / very fast)</t>
+  </si>
+  <si>
+    <t>We'd need to figure out the maximum step size we can take for very fast, then just run that as quickly as we can.  Might end up being 1000 steps per frame or something which wouldn't go as fast was we want</t>
+  </si>
+  <si>
+    <t>These are handled as separate layers</t>
+  </si>
+  <si>
+    <t>Add a single meter that display speed, presure etc</t>
+  </si>
+  <si>
+    <t>Send an email to the guy who wrote this and see what he thinks</t>
+  </si>
+  <si>
+    <t>Tracers</t>
+  </si>
+  <si>
+    <t>Flow lines</t>
+  </si>
+  <si>
+    <t>Reduced the draw time from 4ms to 1ms (just cached some values)</t>
+  </si>
+  <si>
+    <t>Sort out the boundary conditions</t>
+  </si>
+  <si>
+    <t>Just cleaned up a little</t>
+  </si>
+  <si>
+    <t>V0.5.1</t>
+  </si>
+  <si>
+    <t>Put helpful functions in a helper doc</t>
+  </si>
+  <si>
+    <t>Move LBE code off into a separate solver</t>
+  </si>
+  <si>
+    <t>I still access it's private variables from time to time, but atleast now I can see where I'm doing it.</t>
+  </si>
+  <si>
+    <t>Abstract out the LBE solver</t>
+  </si>
+  <si>
+    <t>Can 'push' fluid</t>
+  </si>
+  <si>
+    <t>Can remove barriers</t>
+  </si>
+  <si>
+    <t>Can add barries with mouse</t>
+  </si>
+  <si>
+    <t>Put fluiddynamics stuff into a class</t>
+  </si>
+  <si>
+    <t>(plus remove everything you can)</t>
   </si>
 </sst>
 </file>
@@ -361,7 +445,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -400,14 +484,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -722,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,20 +833,20 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="22"/>
+      <c r="A2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
+      <c r="A3" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -828,19 +911,19 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -931,7 +1014,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -943,24 +1026,24 @@
         <v>4</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="A19" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
+      <c r="A20" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,7 +1054,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -983,7 +1066,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -995,10 +1078,10 @@
         <v>4</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,24 +1092,24 @@
         <v>4</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="A26" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,10 +1120,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,10 +1134,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1064,11 +1147,11 @@
       <c r="B29" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>54</v>
+      <c r="C29" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1078,8 +1161,8 @@
       <c r="B30" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>55</v>
+      <c r="C30" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -1090,180 +1173,191 @@
       <c r="B31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="23" t="s">
-        <v>56</v>
+      <c r="C31" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>57</v>
-      </c>
+      <c r="A32" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="23"/>
+      <c r="A33" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>7</v>
+      <c r="A34" s="7">
+        <v>42478</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>7</v>
+      <c r="A35" s="7">
+        <v>42478</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>45</v>
-      </c>
+      <c r="A36" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="A37" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="14" t="s">
-        <v>47</v>
+      <c r="A38" s="7">
+        <v>42478</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="7">
+        <v>42478</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="12" t="s">
-        <v>58</v>
+      <c r="A40" s="7">
+        <v>42478</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A46" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="2"/>
+      <c r="A47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
+      <c r="A48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
+      <c r="A49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,30 +1367,43 @@
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="2"/>
+      <c r="A53" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
-      <c r="C55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
-      <c r="C56" s="2"/>
+      <c r="C56" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1306,33 +1413,57 @@
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="2"/>
+      <c r="A58" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="2"/>
+      <c r="A60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="A61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="2"/>
+      <c r="A62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,21 +1473,31 @@
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="2"/>
+      <c r="A64" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="2"/>
+      <c r="A65" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="2"/>
+      <c r="A66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1366,27 +1507,37 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="2"/>
+      <c r="A68" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="2"/>
+      <c r="A69" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="2"/>
+      <c r="A70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>64</v>
+      </c>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="2"/>
+      <c r="C71" s="14"/>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,39 +1553,75 @@
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="2"/>
+      <c r="A74" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="2"/>
+      <c r="A75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="A76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="A77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1503,20 +1690,127 @@
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A49:C49"/>
+  <mergeCells count="23">
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
V0.6 Free form drawing
Can add barries with mouse
Can remove barriers
Change brush size with + and -
Change brush type
Preview the brush
UI for selecting brush type and size
Fixed the (harmless) init bug on page load
Fluid dragging
Hilight selected brush
</commit_message>
<xml_diff>
--- a/cfd todo.xlsx
+++ b/cfd todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -181,9 +181,6 @@
     <t>Use hand to click and drag these parts around</t>
   </si>
   <si>
-    <t>V0.7</t>
-  </si>
-  <si>
     <t>Free form drawing</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>In this mode fluid comes out of founts and into wells, and the edges either solid or infinate</t>
   </si>
   <si>
-    <t>V0.6.5</t>
-  </si>
-  <si>
     <t>Instruments</t>
   </si>
   <si>
@@ -265,9 +259,6 @@
     <t>Abstract out the LBE solver</t>
   </si>
   <si>
-    <t>Can 'push' fluid</t>
-  </si>
-  <si>
     <t>Can remove barriers</t>
   </si>
   <si>
@@ -278,6 +269,48 @@
   </si>
   <si>
     <t>(plus remove everything you can)</t>
+  </si>
+  <si>
+    <t>V0.7.2</t>
+  </si>
+  <si>
+    <t>V0.7.1</t>
+  </si>
+  <si>
+    <t>Via shift</t>
+  </si>
+  <si>
+    <t>Line, circle, square</t>
+  </si>
+  <si>
+    <t>Change brush type</t>
+  </si>
+  <si>
+    <t>Change brush size with + and -</t>
+  </si>
+  <si>
+    <t>Just blend 50% white or something</t>
+  </si>
+  <si>
+    <t>Preview the brush</t>
+  </si>
+  <si>
+    <t>UI for selecting brush type and size</t>
+  </si>
+  <si>
+    <t>Have presure as one of the options to show</t>
+  </si>
+  <si>
+    <t>Fixed the (harmless) init bug on page load</t>
+  </si>
+  <si>
+    <t>Fluid dragging</t>
+  </si>
+  <si>
+    <t>Both adding from left side, and place with mouse</t>
+  </si>
+  <si>
+    <t>Hilight selected brush in bile</t>
   </si>
 </sst>
 </file>
@@ -805,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,10 +1235,10 @@
         <v>4</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,12 +1252,12 @@
         <v>39</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -1232,7 +1265,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -1246,10 +1279,10 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1260,7 +1293,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D39" s="2"/>
     </row>
@@ -1272,333 +1305,373 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="2"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="14"/>
+      <c r="A42" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="14"/>
+      <c r="A43" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="14"/>
+      <c r="A44" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="2"/>
+      <c r="A45" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>42480</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="21" t="s">
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="s">
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="2" t="s">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
@@ -1608,7 +1681,7 @@
         <v>7</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D78" s="2"/>
     </row>
@@ -1619,27 +1692,49 @@
       <c r="B79" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D79" s="2"/>
+      <c r="C79" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="A80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="2"/>
+      <c r="A81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="2"/>
+      <c r="A82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,31 +1881,49 @@
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
     </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A55:C55"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A61:C61"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A53:C53"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A72:C72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
V1.0 fit and finish Added experimental support for gravity Added headers on JS files including origional credit. Contrast slider Don’t draw outside 2 cells of simulation Add gravity button Remove tracers that end up stuck on the bottom / top Polish up the UI
</commit_message>
<xml_diff>
--- a/cfd todo.xlsx
+++ b/cfd todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Add sensor</t>
   </si>
   <si>
-    <t>In this mode fluid comes out of inlets and into outlets and the edges either solid or infinate</t>
-  </si>
-  <si>
     <t>V0.7</t>
   </si>
   <si>
@@ -298,15 +295,6 @@
     <t>Load preset layouts from XML</t>
   </si>
   <si>
-    <t>Inlets and outlets</t>
-  </si>
-  <si>
-    <t>Can be on the same layer as barriers.  Just change this to something else like 'attribute' or something</t>
-  </si>
-  <si>
-    <t>0 = none, 1= barrier, 2 = inlet, 3= outlet</t>
-  </si>
-  <si>
     <t>Switch barriers from true/false to 0/1</t>
   </si>
   <si>
@@ -334,9 +322,6 @@
     <t>Polish up the UI</t>
   </si>
   <si>
-    <t>Fix any remaining bugs</t>
-  </si>
-  <si>
     <t>Have UI update when loading experiments</t>
   </si>
   <si>
@@ -379,9 +364,6 @@
     <t>bullet, wedge, aero foil etc</t>
   </si>
   <si>
-    <t>Add disclaimer to javascript allowing usage.</t>
-  </si>
-  <si>
     <t>Add viscosity back in.</t>
   </si>
   <si>
@@ -419,6 +401,144 @@
   </si>
   <si>
     <t>Would need to measure water flow (sensor?) and be able to reverse tunnel direction</t>
+  </si>
+  <si>
+    <t>Add license  to javascript allowing usage as per origional license</t>
+  </si>
+  <si>
+    <t>Just reduce the step size if this occurs</t>
+  </si>
+  <si>
+    <t>Automatical step size reduction</t>
+  </si>
+  <si>
+    <t>Various speed modes, 1x, 10x, 0.1x</t>
+  </si>
+  <si>
+    <t>Add contrast back in</t>
+  </si>
+  <si>
+    <t>Better handling of instability</t>
+  </si>
+  <si>
+    <t>Tracers working with 0 tunnel speed</t>
+  </si>
+  <si>
+    <t>Sticks and balls (to measure velicity and curl)</t>
+  </si>
+  <si>
+    <t>Friction on barriers</t>
+  </si>
+  <si>
+    <t>Speed in center of pipe vs edges</t>
+  </si>
+  <si>
+    <t>Need edge barriers for this, also might need friction (but it seems to work anyway?)</t>
+  </si>
+  <si>
+    <t>Whirlpool</t>
+  </si>
+  <si>
+    <t>Control over how the inlets / outlets work</t>
+  </si>
+  <si>
+    <t>I.e. presure or something?</t>
+  </si>
+  <si>
+    <t>I just give them random locations</t>
+  </si>
+  <si>
+    <t>UI to switch between barriers, inlets, and outlets</t>
+  </si>
+  <si>
+    <t>I think I'm just reseting, but it locks up for some reason?</t>
+  </si>
+  <si>
+    <t>Add time scale settings</t>
+  </si>
+  <si>
+    <t>1x, 10x, 0.1x</t>
+  </si>
+  <si>
+    <t>Create some more experiments</t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <t>Play things</t>
+  </si>
+  <si>
+    <t>V1.2</t>
+  </si>
+  <si>
+    <t>Internals</t>
+  </si>
+  <si>
+    <t>Added inlets and outlets</t>
+  </si>
+  <si>
+    <t>This took ages and then I realised I just set the density with setEqualibrium</t>
+  </si>
+  <si>
+    <t>Don’t draw outside 2 cells of simulation</t>
+  </si>
+  <si>
+    <t>These are needed for simulation right?</t>
+  </si>
+  <si>
+    <t>Remove tracers that end up stuck on the bottom / top</t>
+  </si>
+  <si>
+    <t>Try to get units in there</t>
+  </si>
+  <si>
+    <t>I.e. gravity at 10 m/s and stuff.</t>
+  </si>
+  <si>
+    <t>Variable density</t>
+  </si>
+  <si>
+    <t>Seems to work, but doesn't make much difference</t>
+  </si>
+  <si>
+    <t>Contrast slider</t>
+  </si>
+  <si>
+    <t>Polish experiment 1</t>
+  </si>
+  <si>
+    <t>Polish experiment 2</t>
+  </si>
+  <si>
+    <t>Polish experiment 3</t>
+  </si>
+  <si>
+    <t>Polish experiment 5</t>
+  </si>
+  <si>
+    <t>Polish experiment 4</t>
+  </si>
+  <si>
+    <t>Added experimental support for gravity</t>
+  </si>
+  <si>
+    <t>Added headers on JS files including origional credit.</t>
+  </si>
+  <si>
+    <t>Add gravity button</t>
+  </si>
+  <si>
+    <t>Maybe just on / off for the moment.</t>
+  </si>
+  <si>
+    <t>Extra experiments</t>
+  </si>
+  <si>
+    <t>V1.3</t>
+  </si>
+  <si>
+    <t>And more generaly when using keyboard shortcuts</t>
   </si>
 </sst>
 </file>
@@ -490,7 +610,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -578,6 +698,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -586,7 +719,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -626,6 +759,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -946,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:D91"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,19 +1110,19 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1052,19 +1188,19 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,19 +1308,19 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,19 +1374,19 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1320,19 +1456,19 @@
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1364,19 +1500,19 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,19 +1562,19 @@
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,19 +1698,19 @@
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
+      <c r="A54" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,19 +1770,19 @@
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1657,10 +1793,10 @@
         <v>4</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,7 +1807,7 @@
         <v>4</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D64" s="2"/>
     </row>
@@ -1683,7 +1819,7 @@
         <v>4</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D65" s="2"/>
     </row>
@@ -1695,10 +1831,10 @@
         <v>4</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1709,7 +1845,7 @@
         <v>4</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D67" s="2"/>
     </row>
@@ -1721,7 +1857,7 @@
         <v>4</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D68" s="2"/>
     </row>
@@ -1733,7 +1869,7 @@
         <v>4</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D69" s="2"/>
     </row>
@@ -1745,7 +1881,7 @@
         <v>4</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -1757,10 +1893,10 @@
         <v>4</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1771,7 +1907,7 @@
         <v>4</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D72" s="2"/>
     </row>
@@ -1783,10 +1919,10 @@
         <v>4</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1797,7 +1933,7 @@
         <v>4</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -1809,7 +1945,7 @@
         <v>4</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D75" s="2"/>
     </row>
@@ -1821,10 +1957,10 @@
         <v>4</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,242 +1971,220 @@
         <v>4</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>120</v>
-      </c>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B80" s="21"/>
-      <c r="C80" s="21"/>
+      <c r="A80" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
+        <v>42482</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C82" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>94</v>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
+        <v>42482</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
+        <v>42482</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>135</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E83" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
-      <c r="C84" s="14" t="s">
-        <v>121</v>
-      </c>
+      <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="2"/>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B86" s="21"/>
-      <c r="C86" s="21"/>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B86" s="25"/>
+      <c r="C86" s="25"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="B87" s="22"/>
-      <c r="C87" s="22"/>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
+        <v>42485</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>7</v>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
+        <v>42485</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>7</v>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
+        <v>42485</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>7</v>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
+        <v>42485</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="11" t="s">
-        <v>116</v>
+        <v>155</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
+        <v>42485</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="2"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
+        <v>42485</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
+        <v>42485</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>59</v>
-      </c>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C95" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>61</v>
-      </c>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="A99" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="A100" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
@@ -2080,9 +2194,11 @@
         <v>7</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D101" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
@@ -2091,11 +2207,11 @@
       <c r="B102" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>126</v>
+      <c r="C102" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2105,125 +2221,193 @@
       <c r="B103" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D103" s="2" t="s">
+      <c r="C103" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="14" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4"/>
-      <c r="C105" s="2"/>
       <c r="D105" s="2"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="2"/>
+      <c r="A106" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="23" t="s">
+        <v>163</v>
+      </c>
       <c r="D106" s="2"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="2"/>
+      <c r="A107" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" s="23" t="s">
+        <v>164</v>
+      </c>
       <c r="D107" s="2"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="2"/>
+      <c r="A108" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="23" t="s">
+        <v>165</v>
+      </c>
       <c r="D108" s="2"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="2"/>
+      <c r="A109" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="23" t="s">
+        <v>167</v>
+      </c>
       <c r="D109" s="2"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="2"/>
+      <c r="A110" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" s="23" t="s">
+        <v>166</v>
+      </c>
       <c r="D110" s="2"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="2"/>
+      <c r="C111" s="21"/>
       <c r="D111" s="2"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="2"/>
+      <c r="A112" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B112" s="24"/>
+      <c r="C112" s="24"/>
       <c r="D112" s="2"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="2"/>
+      <c r="A113" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B113" s="25"/>
+      <c r="C113" s="25"/>
       <c r="D113" s="2"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="B114" s="21"/>
-      <c r="C114" s="21"/>
+      <c r="A114" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" s="22" t="s">
+        <v>136</v>
+      </c>
       <c r="D114" s="2"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="4"/>
-      <c r="B115" s="4"/>
-      <c r="C115" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="A115" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D115" s="2"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="4"/>
-      <c r="B116" s="4"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
+      <c r="A116" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
-      <c r="C117" s="2"/>
+      <c r="C117" s="22"/>
       <c r="D117" s="2"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="2"/>
+      <c r="A118" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B118" s="24"/>
+      <c r="C118" s="24"/>
       <c r="D118" s="2"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="4"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="2"/>
+      <c r="A119" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B119" s="25"/>
+      <c r="C119" s="25"/>
       <c r="D119" s="2"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
+      <c r="C120" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
-      <c r="C121" s="2"/>
+      <c r="C121" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="D121" s="2"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2233,35 +2417,323 @@
       <c r="D122" s="2"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
-      <c r="B123" s="4"/>
-      <c r="C123" s="2"/>
+      <c r="A123" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B123" s="24"/>
+      <c r="C123" s="24"/>
       <c r="D123" s="2"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
-      <c r="B124" s="4"/>
-      <c r="C124" s="2"/>
+      <c r="A124" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D124" s="2"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
-      <c r="B125" s="4"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
+      <c r="A125" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D127" s="2"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D131" s="2"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4"/>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B144" s="24"/>
+      <c r="C144" s="24"/>
+      <c r="D144" s="2"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
+      <c r="C145" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="4"/>
+      <c r="B147" s="4"/>
+      <c r="C147" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D147" s="2"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="4"/>
+      <c r="B148" s="4"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A114:C114"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A36:C36"/>
+  <mergeCells count="30">
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A100:C100"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A19:C19"/>
@@ -2269,13 +2741,27 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A144:C144"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A55:C55"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A123:C123"/>
+    <mergeCell ref="A79:C79"/>
     <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="A85:C85"/>
     <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="A112:C112"/>
+    <mergeCell ref="A113:C113"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="A119:C119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>